<commit_message>
fix lady aleera bamboozel random algorithmus
</commit_message>
<xml_diff>
--- a/documents/Arten von Kills.xlsx
+++ b/documents/Arten von Kills.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steve\Programme\Java\Werwolf\src\documents\2_7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\IdeaProjects\Werwolf\src\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9BB10C9-4FAB-4FD9-8B74-7511320042B5}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7485" xr2:uid="{FFF739EF-B70A-41AA-8CCA-B8E82F2D4968}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7488"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -68,7 +67,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -427,19 +426,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A825FFC5-EFB8-4F04-9F1D-9AFB0D95370F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="6" width="13.28515625" customWidth="1"/>
+    <col min="2" max="6" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -456,7 +455,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -476,7 +475,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -496,7 +495,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -516,7 +515,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>

</xml_diff>